<commit_message>
new 5 scripts are added
</commit_message>
<xml_diff>
--- a/OnedaycartMaven/src/test/java/commonData/emails.xlsx
+++ b/OnedaycartMaven/src/test/java/commonData/emails.xlsx
@@ -4,19 +4,19 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="135" windowWidth="14355" windowHeight="4695" activeTab="1"/>
+    <workbookView xWindow="360" yWindow="135" windowWidth="14355" windowHeight="4695" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="email" sheetId="1" r:id="rId1"/>
     <sheet name="chat" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="address" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>emails</t>
   </si>
@@ -45,7 +45,49 @@
     <t>pavandpagal@gmail.com</t>
   </si>
   <si>
-    <t>fghsafgf</t>
+    <t>add more products</t>
+  </si>
+  <si>
+    <t>Mobile no</t>
+  </si>
+  <si>
+    <t>land phone</t>
+  </si>
+  <si>
+    <t>street1</t>
+  </si>
+  <si>
+    <t>street2</t>
+  </si>
+  <si>
+    <t>city</t>
+  </si>
+  <si>
+    <t>postal code</t>
+  </si>
+  <si>
+    <t>land mark</t>
+  </si>
+  <si>
+    <t>Munnar</t>
+  </si>
+  <si>
+    <t>church</t>
+  </si>
+  <si>
+    <t>KEB</t>
+  </si>
+  <si>
+    <t>lane</t>
+  </si>
+  <si>
+    <t>997287893</t>
+  </si>
+  <si>
+    <t>8310342658</t>
+  </si>
+  <si>
+    <t>682001</t>
   </si>
 </sst>
 </file>
@@ -92,9 +134,10 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -426,8 +469,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -464,12 +507,65 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>